<commit_message>
fix: drop pypdf2 dependency
Dropping pypdf2 dependency as merging can be achieved with matplotlib
with the pdf backend.

Also fixed an issue where fonts were not loaded correctly.
</commit_message>
<xml_diff>
--- a/examples/example/example.xlsx
+++ b/examples/example/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/007f372e7d4f37f7/Zeilschool/Shit Happens - ZSN expansion/examples/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\siemdejong\ithappens\examples\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{FCFE40BA-DE3D-475A-93FF-4C6BFB0F8563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B986A03-3CCF-42B4-AF8A-4EDA16EC5A7C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13241B44-25C5-4854-BF83-35343A8DFAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="1370" windowWidth="19420" windowHeight="10300" xr2:uid="{19652FEE-D4C3-46F0-84E0-181B38667A7D}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11505" xr2:uid="{19652FEE-D4C3-46F0-84E0-181B38667A7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>desc</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>misery_index</t>
+  </si>
+  <si>
+    <t>This is just an example</t>
   </si>
 </sst>
 </file>
@@ -84,7 +87,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -99,12 +102,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -400,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE463B05-8062-4172-92A5-06C98D47A8DD}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C47"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,6 +426,14 @@
         <v>80</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: force the use of input column headers
To make it as obvious as possible.

BREAKING CHANGE: any previous input formats with random header names
won't work anymore.
</commit_message>
<xml_diff>
--- a/examples/example/example.xlsx
+++ b/examples/example/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\siemdejong\ithappens\examples\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13241B44-25C5-4854-BF83-35343A8DFAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941D48C6-10CD-4664-ADCC-7FBABE91A194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11505" xr2:uid="{19652FEE-D4C3-46F0-84E0-181B38667A7D}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11505" xr2:uid="{19652FEE-D4C3-46F0-84E0-181B38667A7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -38,16 +38,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>desc</t>
-  </si>
-  <si>
     <t>You don't know how to use this tool</t>
   </si>
   <si>
-    <t>misery_index</t>
+    <t>This is just an example</t>
   </si>
   <si>
-    <t>This is just an example</t>
+    <t>situation</t>
+  </si>
+  <si>
+    <t>misery index</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,15 +412,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>80</v>
@@ -428,7 +428,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>

</xml_diff>

<commit_message>
feat: add front image
fixes #2
</commit_message>
<xml_diff>
--- a/examples/example/example.xlsx
+++ b/examples/example/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\siemdejong\ithappens\examples\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941D48C6-10CD-4664-ADCC-7FBABE91A194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3238E7-9737-44F5-8683-074058C63448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11505" xr2:uid="{19652FEE-D4C3-46F0-84E0-181B38667A7D}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11505" xr2:uid="{19652FEE-D4C3-46F0-84E0-181B38667A7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>You don't know how to use this tool</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>misery index</t>
+  </si>
+  <si>
+    <t>simple stick figure.png</t>
+  </si>
+  <si>
+    <t>umbrella.png</t>
+  </si>
+  <si>
+    <t>image</t>
   </si>
 </sst>
 </file>
@@ -399,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE463B05-8062-4172-92A5-06C98D47A8DD}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,31 +419,41 @@
     <col min="1" max="1" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>80</v>
       </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>